<commit_message>
kalo gw malu tuh
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,60 +436,34 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>nama</t>
+          <t>aca</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>kelas</t>
+          <t>aja</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>aoa</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rian</t>
+          <t>aca</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>12</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>endang</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>riski</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>jaki</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>10</t>
+          <t>aja</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>aoa</t>
         </is>
       </c>
     </row>

</xml_diff>